<commit_message>
Update check if term status is false to prevent assignments when user import
</commit_message>
<xml_diff>
--- a/TeachingAssignmentManagement/Uploads/CNTT UIS-ThoiKhoaBieu_TieuChuan_Mau.xlsx
+++ b/TeachingAssignmentManagement/Uploads/CNTT UIS-ThoiKhoaBieu_TieuChuan_Mau.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\duy94\Downloads\Excel dữ liệu\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5770754-C655-418B-996A-929EAF074E64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{544B42B4-5AB5-4D02-8CCF-F27DF531BBAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5760" yWindow="3360" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TIÊU CHUẨN- phân công GV K28" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9666" uniqueCount="864">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9665" uniqueCount="864">
   <si>
     <t>MaGocLHP</t>
   </si>
@@ -6349,10 +6349,10 @@
   <dimension ref="A1:AF312"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="Y2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="G13" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AE2" sqref="AE2"/>
+      <selection pane="bottomRight" activeCell="P26" sqref="P26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8820,9 +8820,7 @@
       <c r="O26" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="P26" s="11" t="s">
-        <v>38</v>
-      </c>
+      <c r="P26" s="11"/>
       <c r="Q26" s="11" t="s">
         <v>140</v>
       </c>

</xml_diff>